<commit_message>
Submit to JLC for assembly
</commit_message>
<xml_diff>
--- a/Rev2_F401RE/eagle/revb_BOM.xlsx
+++ b/Rev2_F401RE/eagle/revb_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wpi0-my.sharepoint.com/personal/jwbuchta_wpi_edu/Documents/Projects/Interrupter/TeslaCoilController/Rev2_F401RE/eagle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{6E2CAA61-36B4-4ECB-9F70-2D9154124FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{567628B2-C123-423D-B18E-1B330EF77D20}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{6E2CAA61-36B4-4ECB-9F70-2D9154124FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88FB8E93-C572-43DF-B4A2-5D81A5B408F8}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{D47F748F-FF22-4AD5-A6FA-A0F321CBB47E}"/>
+    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="9984" xr2:uid="{D47F748F-FF22-4AD5-A6FA-A0F321CBB47E}"/>
   </bookViews>
   <sheets>
     <sheet name="revb_BOM" sheetId="1" r:id="rId1"/>
@@ -1373,13 +1373,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E12622-1509-4756-8C38-8BF3F9E042CF}">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="13.5234375" customWidth="1"/>
+    <col min="2" max="2" width="18.68359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.3125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7890625" customWidth="1"/>
     <col min="5" max="5" width="117.41796875" bestFit="1" customWidth="1"/>

</xml_diff>